<commit_message>
Converted to use ExampleReviewExcel
</commit_message>
<xml_diff>
--- a/ExampleReviewExcel.xlsx
+++ b/ExampleReviewExcel.xlsx
@@ -1053,7 +1053,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="10" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1101,7 +1101,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="10" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1187,11 +1187,11 @@
   </sheetPr>
   <dimension ref="A1:HR8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V6" activeCellId="0" sqref="V6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.67"/>
@@ -2145,7 +2145,7 @@
         <v>1</v>
       </c>
       <c r="V3" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3" s="10" t="n">
         <v>4</v>
@@ -2339,14 +2339,22 @@
       <c r="HF3" s="11"/>
       <c r="HG3" s="11"/>
       <c r="HH3" s="11"/>
-      <c r="HI3" s="13"/>
-      <c r="HJ3" s="11"/>
-      <c r="HK3" s="11"/>
-      <c r="HL3" s="11"/>
-      <c r="HM3" s="11"/>
-      <c r="HN3" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="HI3" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="HJ3" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="HK3" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="HL3" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="HM3" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="HN3" s="10"/>
       <c r="HO3" s="14" t="n">
         <v>111</v>
       </c>
@@ -2396,7 +2404,7 @@
         <v>1</v>
       </c>
       <c r="V4" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4" s="10" t="n">
         <v>4</v>
@@ -2518,10 +2526,22 @@
       <c r="HC4" s="11"/>
       <c r="HD4" s="11"/>
       <c r="HE4" s="10"/>
-      <c r="HI4" s="13"/>
-      <c r="HN4" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="HI4" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="HJ4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HK4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HL4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HM4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HN4" s="10"/>
       <c r="HO4" s="14" t="n">
         <v>5</v>
       </c>
@@ -2569,7 +2589,7 @@
         <v>0</v>
       </c>
       <c r="V5" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5" s="10" t="n">
         <v>2</v>
@@ -2689,10 +2709,22 @@
       <c r="HC5" s="11"/>
       <c r="HD5" s="11"/>
       <c r="HE5" s="10"/>
-      <c r="HI5" s="13"/>
-      <c r="HN5" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="HI5" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="HJ5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HK5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HL5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HM5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HN5" s="10"/>
       <c r="HO5" s="14" t="n">
         <v>149</v>
       </c>
@@ -2857,7 +2889,21 @@
       <c r="HC6" s="11"/>
       <c r="HD6" s="11"/>
       <c r="HE6" s="10"/>
-      <c r="HI6" s="13"/>
+      <c r="HI6" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="HJ6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HK6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HL6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HM6" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="HN6" s="10"/>
       <c r="HO6" s="14" t="n">
         <v>0</v>
@@ -3095,6 +3141,15 @@
       <c r="HJ7" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="HK7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HL7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HM7" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="HN7" s="10"/>
       <c r="HO7" s="14" t="n">
         <v>25</v>
@@ -3353,7 +3408,18 @@
       <c r="HJ8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="HN8" s="10"/>
+      <c r="HK8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HL8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HM8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="HN8" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="HO8" s="14" t="n">
         <v>105</v>
       </c>

</xml_diff>